<commit_message>
Fix using queries with selects
</commit_message>
<xml_diff>
--- a/form-files/tables/selects/forms/selects/selects.xlsx
+++ b/form-files/tables/selects/forms/selects/selects.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="60" windowWidth="37760" windowHeight="13600"/>
+    <workbookView xWindow="5140" yWindow="100" windowWidth="38040" windowHeight="21420"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="116">
   <si>
     <t>comments</t>
   </si>
@@ -271,111 +271,118 @@
   </si>
   <si>
     <t>"https://query.yahooapis.com/v1/public/yql?format=json&amp;q=" +  encodeURIComponent("select * from geo.countries where place='North America'")</t>
+  </si>
+  <si>
+    <t>states</t>
+  </si>
+  <si>
+    <t>"https://query.yahooapis.com/v1/public/yql?format=json&amp;q=" +  encodeURIComponent("select * from geo.states where place='" + data('country') + "'")</t>
+  </si>
+  <si>
+    <t>regions_csv</t>
+  </si>
+  <si>
+    <t>"regions.csv"</t>
+  </si>
+  <si>
+    <t>countries_csv</t>
+  </si>
+  <si>
+    <t>content_provider_test</t>
+  </si>
+  <si>
+    <t>"content://org.opendatakit.FileContentProviderExample/"</t>
+  </si>
+  <si>
+    <t>context</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>form_id</t>
+  </si>
+  <si>
+    <t>selects</t>
+  </si>
+  <si>
+    <t>form_version</t>
+  </si>
+  <si>
+    <t>Select Examples</t>
+  </si>
+  <si>
+    <t>setting_name</t>
+  </si>
+  <si>
+    <t>display.title</t>
+  </si>
+  <si>
+    <t>survey</t>
+  </si>
+  <si>
+    <t>query_name</t>
+  </si>
+  <si>
+    <t>choice_list_name</t>
+  </si>
+  <si>
+    <t>data_value</t>
+  </si>
+  <si>
+    <t>display.image</t>
+  </si>
+  <si>
+    <t>display.text</t>
+  </si>
+  <si>
+    <t>clause</t>
+  </si>
+  <si>
+    <t>if</t>
+  </si>
+  <si>
+    <t>end if</t>
+  </si>
+  <si>
+    <t>display.hint</t>
+  </si>
+  <si>
+    <t>values_list</t>
+  </si>
+  <si>
+    <t>select_one</t>
+  </si>
+  <si>
+    <t>select_one_with_other</t>
+  </si>
+  <si>
+    <t>hideInContents</t>
   </si>
   <si>
     <t>context.query.results ? _.map(context.query.results.place, function(place){
 place.label = place.name;
+place.data_value = place.name;
+place.display = {text:place.label};
 return place;
 }) : []</t>
   </si>
   <si>
-    <t>states</t>
-  </si>
-  <si>
-    <t>"https://query.yahooapis.com/v1/public/yql?format=json&amp;q=" +  encodeURIComponent("select * from geo.states where place='" + data('country') + "'")</t>
-  </si>
-  <si>
-    <t>regions_csv</t>
-  </si>
-  <si>
-    <t>"regions.csv"</t>
-  </si>
-  <si>
     <t>_.chain(context).pluck('region').uniq().map(function(region){
-return {name:region, label:region};
+return {name:region, label:region, data_value:region, display:{text:region}};
 }).value()</t>
-  </si>
-  <si>
-    <t>countries_csv</t>
   </si>
   <si>
     <t>_.map(context, function(place){
 place.name = place.country;
 place.label = place.country;
+place.data_value = place.name;
+place.display = {text:place.label};
 return place;
 })</t>
   </si>
   <si>
-    <t>content_provider_test</t>
-  </si>
-  <si>
-    <t>"content://org.opendatakit.FileContentProviderExample/"</t>
-  </si>
-  <si>
-    <t>context</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>form_id</t>
-  </si>
-  <si>
-    <t>selects</t>
-  </si>
-  <si>
-    <t>form_version</t>
-  </si>
-  <si>
-    <t>Select Examples</t>
-  </si>
-  <si>
-    <t>setting_name</t>
-  </si>
-  <si>
-    <t>display.title</t>
-  </si>
-  <si>
-    <t>survey</t>
-  </si>
-  <si>
-    <t>query_name</t>
-  </si>
-  <si>
-    <t>choice_list_name</t>
-  </si>
-  <si>
-    <t>data_value</t>
-  </si>
-  <si>
-    <t>display.image</t>
-  </si>
-  <si>
-    <t>display.text</t>
-  </si>
-  <si>
-    <t>clause</t>
-  </si>
-  <si>
-    <t>if</t>
-  </si>
-  <si>
-    <t>end if</t>
-  </si>
-  <si>
-    <t>display.hint</t>
-  </si>
-  <si>
-    <t>values_list</t>
-  </si>
-  <si>
-    <t>select_one</t>
-  </si>
-  <si>
-    <t>select_one_with_other</t>
-  </si>
-  <si>
-    <t>hideInContents</t>
+    <t>country_csv</t>
   </si>
 </sst>
 </file>
@@ -744,7 +751,7 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -765,7 +772,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -774,7 +781,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -786,16 +793,16 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="K1" t="s">
         <v>6</v>
       </c>
       <c r="L1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1">
@@ -803,7 +810,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>81</v>
@@ -818,10 +825,10 @@
     <row r="3" spans="1:12" ht="15.75" customHeight="1">
       <c r="A3" s="2"/>
       <c r="D3" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H3" t="s">
         <v>10</v>
@@ -841,7 +848,7 @@
     <row r="5" spans="1:12" ht="15.75" customHeight="1">
       <c r="A5" s="2"/>
       <c r="D5" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>48</v>
@@ -859,7 +866,7 @@
     <row r="6" spans="1:12" ht="15.75" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C6" t="s">
         <v>18</v>
@@ -880,13 +887,13 @@
     <row r="8" spans="1:12" ht="15.75" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
@@ -907,7 +914,7 @@
     <row r="11" spans="1:12" ht="15.75" customHeight="1">
       <c r="A11" s="2"/>
       <c r="B11" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1">
@@ -937,7 +944,7 @@
     <row r="15" spans="1:12" ht="15.75" customHeight="1">
       <c r="A15" s="2"/>
       <c r="D15" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>67</v>
@@ -955,7 +962,7 @@
     <row r="16" spans="1:12" ht="15.75" customHeight="1">
       <c r="A16" s="2"/>
       <c r="D16" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>67</v>
@@ -973,7 +980,7 @@
     <row r="17" spans="1:12" ht="15.75" customHeight="1">
       <c r="A17" s="2"/>
       <c r="D17" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>67</v>
@@ -991,7 +998,7 @@
     <row r="18" spans="1:12" ht="15.75" customHeight="1">
       <c r="A18" s="2"/>
       <c r="D18" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>67</v>
@@ -1015,7 +1022,7 @@
     <row r="20" spans="1:12" ht="15.75" customHeight="1">
       <c r="A20" s="2"/>
       <c r="D20" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>72</v>
@@ -1030,7 +1037,7 @@
     <row r="21" spans="1:12" ht="15.75" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C21" t="s">
         <v>36</v>
@@ -1053,13 +1060,13 @@
     <row r="23" spans="1:12" ht="15.75" customHeight="1">
       <c r="A23" s="2"/>
       <c r="B23" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="15.75" customHeight="1">
       <c r="A24" s="2"/>
       <c r="D24" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>67</v>
@@ -1077,10 +1084,10 @@
     <row r="25" spans="1:12" ht="15.75" customHeight="1">
       <c r="A25" s="2"/>
       <c r="D25" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H25" t="s">
         <v>41</v>
@@ -1092,16 +1099,16 @@
     <row r="26" spans="1:12" ht="15.75" customHeight="1">
       <c r="A26" s="2"/>
       <c r="D26" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F26" t="s">
         <v>43</v>
       </c>
       <c r="H26" t="s">
-        <v>8</v>
+        <v>115</v>
       </c>
       <c r="I26" t="s">
         <v>9</v>
@@ -1113,7 +1120,7 @@
     <row r="27" spans="1:12" ht="15.75" customHeight="1">
       <c r="A27" s="2"/>
       <c r="B27" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
@@ -1122,10 +1129,10 @@
     <row r="28" spans="1:12" ht="15.75" customHeight="1">
       <c r="A28" s="2"/>
       <c r="D28" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="H28" t="s">
         <v>45</v>
@@ -1140,7 +1147,7 @@
     <row r="29" spans="1:12" ht="15.75" customHeight="1">
       <c r="A29" s="2"/>
       <c r="B29" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="12.75" customHeight="1">
@@ -1183,16 +1190,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.75" customHeight="1">
       <c r="A1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" t="s">
         <v>103</v>
-      </c>
-      <c r="B1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16.75" customHeight="1">
@@ -1366,7 +1373,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1378,7 +1385,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="34.5" customHeight="1">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B1" t="s">
         <v>79</v>
@@ -1395,51 +1402,51 @@
         <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34.5" customHeight="1">
       <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
         <v>84</v>
       </c>
-      <c r="B3" t="s">
-        <v>85</v>
-      </c>
       <c r="C3" t="s">
-        <v>83</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34.5" customHeight="1">
       <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" t="s">
         <v>86</v>
       </c>
-      <c r="B4" t="s">
-        <v>87</v>
-      </c>
       <c r="C4" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34.5" customHeight="1">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34.5" customHeight="1">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16.25" customHeight="1"/>
@@ -1468,27 +1475,27 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.75" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="16.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B3">
         <v>20130408</v>
@@ -1496,10 +1503,10 @@
     </row>
     <row r="4" spans="1:3" ht="16.75" customHeight="1">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16.75" customHeight="1"/>

</xml_diff>

<commit_message>
Intermediate clean up for selects templates.
</commit_message>
<xml_diff>
--- a/form-files/tables/selects/forms/selects/selects.xlsx
+++ b/form-files/tables/selects/forms/selects/selects.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5140" yWindow="100" windowWidth="38040" windowHeight="21420"/>
+    <workbookView xWindow="5120" yWindow="80" windowWidth="38040" windowHeight="21420" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="queries" sheetId="3" r:id="rId3"/>
     <sheet name="settings" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="152">
   <si>
     <t>comments</t>
   </si>
@@ -66,9 +66,6 @@
     <t>begin screen</t>
   </si>
   <si>
-    <t>grid</t>
-  </si>
-  <si>
     <t>bird</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>Which devices do you use?</t>
   </si>
   <si>
-    <t>inline</t>
-  </si>
-  <si>
     <t>desktop</t>
   </si>
   <si>
@@ -151,9 +145,6 @@
   </si>
   <si>
     <t>Choose a region:</t>
-  </si>
-  <si>
-    <t>dropdown</t>
   </si>
   <si>
     <t>context.region === data('region')</t>
@@ -384,12 +375,129 @@
   <si>
     <t>country_csv</t>
   </si>
+  <si>
+    <t>select_one_grid</t>
+  </si>
+  <si>
+    <t>Selects Demo</t>
+  </si>
+  <si>
+    <t>What is your favorite holiday?</t>
+  </si>
+  <si>
+    <t>holidays</t>
+  </si>
+  <si>
+    <t>favoriteHoliday</t>
+  </si>
+  <si>
+    <t>select_one_inline</t>
+  </si>
+  <si>
+    <t>secondFavoriteHoliday</t>
+  </si>
+  <si>
+    <t>What is your second favorite holiday?</t>
+  </si>
+  <si>
+    <t>select_one_dropdown</t>
+  </si>
+  <si>
+    <t>thirdFavoriteHoliday</t>
+  </si>
+  <si>
+    <t>What is your third favorite holiday?</t>
+  </si>
+  <si>
+    <t>select_multiple</t>
+  </si>
+  <si>
+    <t>select_multiple_inline</t>
+  </si>
+  <si>
+    <t>select_multiple_grid</t>
+  </si>
+  <si>
+    <t>foods</t>
+  </si>
+  <si>
+    <t>Milk</t>
+  </si>
+  <si>
+    <t>Bread</t>
+  </si>
+  <si>
+    <t>Fruit</t>
+  </si>
+  <si>
+    <t>Meat</t>
+  </si>
+  <si>
+    <t>Vegetable</t>
+  </si>
+  <si>
+    <t>milk</t>
+  </si>
+  <si>
+    <t>bread</t>
+  </si>
+  <si>
+    <t>meat</t>
+  </si>
+  <si>
+    <t>fruit</t>
+  </si>
+  <si>
+    <t>vegetable</t>
+  </si>
+  <si>
+    <t>breakfastFood</t>
+  </si>
+  <si>
+    <t>lunchFood</t>
+  </si>
+  <si>
+    <t>dinnerFood</t>
+  </si>
+  <si>
+    <t>What types of food do you eat for breakfast?</t>
+  </si>
+  <si>
+    <t>What types of food do you eat for lunch?</t>
+  </si>
+  <si>
+    <t>What types of food do you eat for dinner?</t>
+  </si>
+  <si>
+    <t>christmas</t>
+  </si>
+  <si>
+    <t>Christmas</t>
+  </si>
+  <si>
+    <t>thanksgiving</t>
+  </si>
+  <si>
+    <t>Thanksgiving</t>
+  </si>
+  <si>
+    <t>easter</t>
+  </si>
+  <si>
+    <t>Easter</t>
+  </si>
+  <si>
+    <t>halloween</t>
+  </si>
+  <si>
+    <t>Halloween</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -400,6 +508,18 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -425,10 +545,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -447,8 +587,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="21">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -748,10 +911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -772,7 +935,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -781,7 +944,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -793,16 +956,16 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K1" t="s">
         <v>6</v>
       </c>
       <c r="L1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1">
@@ -810,10 +973,10 @@
         <v>7</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H2" t="s">
         <v>8</v>
@@ -825,10 +988,10 @@
     <row r="3" spans="1:12" ht="15.75" customHeight="1">
       <c r="A3" s="2"/>
       <c r="D3" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H3" t="s">
         <v>10</v>
@@ -847,38 +1010,35 @@
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1">
       <c r="A5" s="2"/>
-      <c r="D5" s="5" t="s">
-        <v>109</v>
+      <c r="D5" s="6" t="s">
+        <v>113</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" t="s">
         <v>14</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>15</v>
-      </c>
-      <c r="I5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1">
       <c r="A7" s="2"/>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L7" t="b">
         <v>1</v>
@@ -887,25 +1047,25 @@
     <row r="8" spans="1:12" ht="15.75" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1">
       <c r="A10" s="2"/>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L10" t="b">
         <v>1</v>
@@ -914,13 +1074,13 @@
     <row r="11" spans="1:12" ht="15.75" customHeight="1">
       <c r="A11" s="2"/>
       <c r="B11" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1">
       <c r="A12" s="2"/>
       <c r="B12" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" customHeight="1">
@@ -932,10 +1092,10 @@
     <row r="14" spans="1:12" ht="15.75" customHeight="1">
       <c r="A14" s="2"/>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L14" t="b">
         <v>1</v>
@@ -943,115 +1103,103 @@
     </row>
     <row r="15" spans="1:12" ht="15.75" customHeight="1">
       <c r="A15" s="2"/>
-      <c r="D15" s="5" t="s">
-        <v>109</v>
+      <c r="D15" s="6" t="s">
+        <v>118</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" t="s">
         <v>24</v>
-      </c>
-      <c r="H15" t="s">
-        <v>25</v>
-      </c>
-      <c r="I15" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="15.75" customHeight="1">
       <c r="A16" s="2"/>
-      <c r="D16" s="5" t="s">
-        <v>109</v>
+      <c r="D16" s="6" t="s">
+        <v>118</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F16" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="H16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I16" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="15.75" customHeight="1">
       <c r="A17" s="2"/>
-      <c r="D17" s="5" t="s">
-        <v>109</v>
+      <c r="D17" s="6" t="s">
+        <v>118</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="H17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="I17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="15.75" customHeight="1">
       <c r="A18" s="2"/>
-      <c r="D18" s="5" t="s">
-        <v>109</v>
+      <c r="D18" s="6" t="s">
+        <v>118</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="H18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" customHeight="1">
       <c r="A19" s="2"/>
       <c r="B19" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="15.75" customHeight="1">
       <c r="A20" s="2"/>
       <c r="D20" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="15.75" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="15.75" customHeight="1">
       <c r="A22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" t="s">
         <v>35</v>
-      </c>
-      <c r="D22" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" t="s">
-        <v>37</v>
       </c>
       <c r="L22" t="b">
         <v>1</v>
@@ -1060,67 +1208,64 @@
     <row r="23" spans="1:12" ht="15.75" customHeight="1">
       <c r="A23" s="2"/>
       <c r="B23" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="15.75" customHeight="1">
       <c r="A24" s="2"/>
       <c r="D24" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G24" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24" t="s">
+        <v>37</v>
+      </c>
+      <c r="I24" t="s">
         <v>38</v>
-      </c>
-      <c r="H24" t="s">
-        <v>39</v>
-      </c>
-      <c r="I24" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15.75" customHeight="1">
       <c r="A25" s="2"/>
       <c r="D25" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I25" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="15.75" customHeight="1">
       <c r="A26" s="2"/>
-      <c r="D26" s="5" t="s">
-        <v>109</v>
+      <c r="D26" s="6" t="s">
+        <v>121</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="F26" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="H26" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="I26" t="s">
         <v>9</v>
       </c>
       <c r="K26" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="15.75" customHeight="1">
       <c r="A27" s="2"/>
       <c r="B27" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
@@ -1129,44 +1274,144 @@
     <row r="28" spans="1:12" ht="15.75" customHeight="1">
       <c r="A28" s="2"/>
       <c r="D28" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H28" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I28" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J28" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1">
       <c r="A29" s="2"/>
       <c r="B29" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="12.75" customHeight="1">
       <c r="A30" s="2"/>
+      <c r="B30" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="31" spans="1:12" ht="12.75" customHeight="1">
       <c r="A31" s="2"/>
+      <c r="D31" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" t="s">
+        <v>114</v>
+      </c>
+      <c r="L31" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:12" ht="12.75" customHeight="1">
       <c r="A32" s="2"/>
-    </row>
-    <row r="33" spans="1:1" ht="12.75" customHeight="1">
+      <c r="D32" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H32" t="s">
+        <v>117</v>
+      </c>
+      <c r="I32" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="12.75" customHeight="1">
       <c r="A33" s="2"/>
-    </row>
-    <row r="34" spans="1:1" ht="12.75" customHeight="1">
+      <c r="D33" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H33" t="s">
+        <v>119</v>
+      </c>
+      <c r="I33" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="12.75" customHeight="1">
       <c r="A34" s="2"/>
+      <c r="D34" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H34" t="s">
+        <v>122</v>
+      </c>
+      <c r="I34" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A35" s="2"/>
+      <c r="D35" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="H35" t="s">
+        <v>138</v>
+      </c>
+      <c r="I35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A36" s="2"/>
+      <c r="D36" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="H36" t="s">
+        <v>139</v>
+      </c>
+      <c r="I36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A37" s="2"/>
+      <c r="D37" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="H37" t="s">
+        <v>140</v>
+      </c>
+      <c r="I37" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="12.75" customHeight="1">
+      <c r="A38" s="2"/>
+      <c r="B38" s="4" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1177,10 +1422,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1190,176 +1435,277 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.75" customHeight="1">
       <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" t="s">
         <v>100</v>
-      </c>
-      <c r="B1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16.75" customHeight="1">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.75" customHeight="1">
       <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
         <v>48</v>
       </c>
-      <c r="B3" t="s">
-        <v>51</v>
-      </c>
       <c r="C3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.75" customHeight="1">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.75" customHeight="1">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.75" customHeight="1">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.75" customHeight="1">
       <c r="A7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16.75" customHeight="1">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16.75" customHeight="1">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16.75" customHeight="1">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16.75" customHeight="1"/>
     <row r="12" spans="1:4" ht="16.75" customHeight="1">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D12" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16.75" customHeight="1">
       <c r="A13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" t="s">
         <v>67</v>
       </c>
-      <c r="B13" t="s">
-        <v>70</v>
-      </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16.75" customHeight="1"/>
     <row r="15" spans="1:4" ht="16.75" customHeight="1">
       <c r="A15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16.75" customHeight="1">
       <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" t="s">
         <v>72</v>
       </c>
-      <c r="B16" t="s">
-        <v>75</v>
-      </c>
       <c r="D16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16.75" customHeight="1">
       <c r="A17" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="16.75" customHeight="1"/>
+    <row r="19" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" t="s">
+        <v>144</v>
+      </c>
+      <c r="D19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B20" t="s">
+        <v>146</v>
+      </c>
+      <c r="D20" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A21" t="s">
+        <v>116</v>
+      </c>
+      <c r="B21" t="s">
+        <v>148</v>
+      </c>
+      <c r="D21" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A22" t="s">
+        <v>116</v>
+      </c>
+      <c r="B22" t="s">
+        <v>150</v>
+      </c>
+      <c r="D22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A24" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" t="s">
+        <v>133</v>
+      </c>
+      <c r="D24" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A25" t="s">
+        <v>127</v>
+      </c>
+      <c r="B25" t="s">
+        <v>134</v>
+      </c>
+      <c r="D25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A26" t="s">
+        <v>127</v>
+      </c>
+      <c r="B26" t="s">
+        <v>136</v>
+      </c>
+      <c r="D26" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A27" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" t="s">
+        <v>137</v>
+      </c>
+      <c r="D27" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="12.75" customHeight="1">
+      <c r="A28" t="s">
+        <v>127</v>
+      </c>
+      <c r="B28" t="s">
+        <v>135</v>
+      </c>
+      <c r="D28" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1385,68 +1731,68 @@
   <sheetData>
     <row r="1" spans="1:3" ht="34.5" customHeight="1">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="34.5" customHeight="1">
       <c r="A2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34.5" customHeight="1">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34.5" customHeight="1">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="34.5" customHeight="1">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="34.5" customHeight="1">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16.25" customHeight="1"/>
@@ -1475,27 +1821,27 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.75" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="16.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B3">
         <v>20130408</v>
@@ -1503,10 +1849,10 @@
     </row>
     <row r="4" spans="1:3" ht="16.75" customHeight="1">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16.75" customHeight="1"/>

</xml_diff>

<commit_message>
Clean up of selects with updated formDefs
</commit_message>
<xml_diff>
--- a/form-files/tables/selects/forms/selects/selects.xlsx
+++ b/form-files/tables/selects/forms/selects/selects.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5120" yWindow="80" windowWidth="38040" windowHeight="21420" activeTab="1"/>
+    <workbookView xWindow="7340" yWindow="7480" windowWidth="38040" windowHeight="21420" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,15 +22,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="155">
   <si>
     <t>comments</t>
   </si>
   <si>
     <t>type</t>
-  </si>
-  <si>
-    <t>appearance</t>
   </si>
   <si>
     <t>inputAttributes.data-type</t>
@@ -379,9 +376,6 @@
     <t>select_one_grid</t>
   </si>
   <si>
-    <t>Selects Demo</t>
-  </si>
-  <si>
     <t>What is your favorite holiday?</t>
   </si>
   <si>
@@ -491,6 +485,21 @@
   </si>
   <si>
     <t>Halloween</t>
+  </si>
+  <si>
+    <t>query_type</t>
+  </si>
+  <si>
+    <t>ajax</t>
+  </si>
+  <si>
+    <t>csv</t>
+  </si>
+  <si>
+    <t>Holidays</t>
+  </si>
+  <si>
+    <t>Food</t>
   </si>
 </sst>
 </file>
@@ -545,8 +554,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -591,7 +604,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -602,6 +615,8 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -612,6 +627,8 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -911,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -924,300 +941,300 @@
     <col min="3" max="3" width="33.33203125" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
     <col min="5" max="5" width="35" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" customWidth="1"/>
-    <col min="8" max="8" width="32.6640625" customWidth="1"/>
-    <col min="9" max="9" width="46" customWidth="1"/>
-    <col min="11" max="11" width="25.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="32.6640625" customWidth="1"/>
+    <col min="8" max="8" width="46" customWidth="1"/>
+    <col min="10" max="10" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" t="s">
+        <v>103</v>
+      </c>
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
-        <v>100</v>
-      </c>
-      <c r="J1" t="s">
-        <v>104</v>
-      </c>
       <c r="K1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="D2" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="H2" t="s">
         <v>8</v>
       </c>
-      <c r="I2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1">
+    </row>
+    <row r="3" spans="1:11" ht="15.75" customHeight="1">
       <c r="A3" s="2"/>
       <c r="D3" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
       </c>
       <c r="H3" t="s">
         <v>10</v>
       </c>
-      <c r="I3" t="s">
+    </row>
+    <row r="4" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1">
+    </row>
+    <row r="5" spans="1:11" ht="15.75" customHeight="1">
       <c r="A5" s="2"/>
       <c r="D5" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
       </c>
       <c r="H5" t="s">
         <v>14</v>
       </c>
-      <c r="I5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1">
+    </row>
+    <row r="6" spans="1:11" ht="15.75" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="15.75" customHeight="1">
       <c r="A7" s="2"/>
       <c r="D7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" t="s">
-        <v>18</v>
-      </c>
-      <c r="L7" t="b">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+      <c r="K7" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1">
+    <row r="8" spans="1:11" ht="15.75" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="15.75" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" customHeight="1">
       <c r="A10" s="2"/>
       <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="I10" t="s">
-        <v>20</v>
-      </c>
-      <c r="L10" t="b">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1">
       <c r="A11" s="2"/>
       <c r="B11" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" customHeight="1">
       <c r="A12" s="2"/>
       <c r="B12" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" customHeight="1">
       <c r="A13" s="2"/>
       <c r="B13" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" customHeight="1">
       <c r="A14" s="2"/>
       <c r="D14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I14" t="s">
-        <v>22</v>
-      </c>
-      <c r="L14" t="b">
+        <v>15</v>
+      </c>
+      <c r="H14" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1">
+    <row r="15" spans="1:11" ht="15.75" customHeight="1">
       <c r="A15" s="2"/>
       <c r="D15" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="G15" t="s">
+        <v>22</v>
       </c>
       <c r="H15" t="s">
         <v>23</v>
       </c>
-      <c r="I15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1">
+    </row>
+    <row r="16" spans="1:11" ht="15.75" customHeight="1">
       <c r="A16" s="2"/>
       <c r="D16" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="G16" t="s">
+        <v>24</v>
       </c>
       <c r="H16" t="s">
         <v>25</v>
       </c>
-      <c r="I16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1">
+    </row>
+    <row r="17" spans="1:11" ht="15.75" customHeight="1">
       <c r="A17" s="2"/>
       <c r="D17" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="G17" t="s">
+        <v>26</v>
       </c>
       <c r="H17" t="s">
         <v>27</v>
       </c>
-      <c r="I17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="15.75" customHeight="1">
+    </row>
+    <row r="18" spans="1:11" ht="15.75" customHeight="1">
       <c r="A18" s="2"/>
       <c r="D18" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="G18" t="s">
+        <v>28</v>
       </c>
       <c r="H18" t="s">
         <v>29</v>
       </c>
-      <c r="I18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="15.75" customHeight="1">
+    </row>
+    <row r="19" spans="1:11" ht="15.75" customHeight="1">
       <c r="A19" s="2"/>
       <c r="B19" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="15.75" customHeight="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" customHeight="1">
       <c r="A20" s="2"/>
       <c r="D20" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
+      </c>
+      <c r="G20" t="s">
+        <v>30</v>
       </c>
       <c r="H20" t="s">
         <v>31</v>
       </c>
-      <c r="I20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="15.75" customHeight="1">
+    </row>
+    <row r="21" spans="1:11" ht="15.75" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A22" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" t="s">
-        <v>16</v>
-      </c>
-      <c r="I22" t="s">
-        <v>35</v>
-      </c>
-      <c r="L22" t="b">
+      <c r="K22" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="15.75" customHeight="1">
+    <row r="23" spans="1:11" ht="15.75" customHeight="1">
       <c r="A23" s="2"/>
       <c r="B23" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" customHeight="1">
       <c r="A24" s="2"/>
       <c r="D24" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="F24" t="s">
+        <v>35</v>
       </c>
       <c r="G24" t="s">
         <v>36</v>
@@ -1225,59 +1242,59 @@
       <c r="H24" t="s">
         <v>37</v>
       </c>
-      <c r="I24" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="15.75" customHeight="1">
+    </row>
+    <row r="25" spans="1:11" ht="15.75" customHeight="1">
       <c r="A25" s="2"/>
       <c r="D25" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
+      </c>
+      <c r="G25" t="s">
+        <v>38</v>
       </c>
       <c r="H25" t="s">
         <v>39</v>
       </c>
-      <c r="I25" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="15.75" customHeight="1">
+    </row>
+    <row r="26" spans="1:11" ht="15.75" customHeight="1">
       <c r="A26" s="2"/>
       <c r="D26" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
+      </c>
+      <c r="G26" t="s">
+        <v>111</v>
       </c>
       <c r="H26" t="s">
-        <v>112</v>
-      </c>
-      <c r="I26" t="s">
-        <v>9</v>
-      </c>
-      <c r="K26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="15.75" customHeight="1">
+        <v>8</v>
+      </c>
+      <c r="J26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" customHeight="1">
       <c r="A27" s="2"/>
       <c r="B27" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15.75" customHeight="1">
+    <row r="28" spans="1:11" ht="15.75" customHeight="1">
       <c r="A28" s="2"/>
       <c r="D28" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+      <c r="G28" t="s">
+        <v>41</v>
       </c>
       <c r="H28" t="s">
         <v>42</v>
@@ -1285,128 +1302,149 @@
       <c r="I28" t="s">
         <v>43</v>
       </c>
-      <c r="J28" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="15.75" customHeight="1">
+    </row>
+    <row r="29" spans="1:11" ht="15.75" customHeight="1">
       <c r="A29" s="2"/>
       <c r="B29" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="12.75" customHeight="1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="12.75" customHeight="1">
       <c r="A30" s="2"/>
       <c r="B30" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="12.75" customHeight="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="12.75" customHeight="1">
       <c r="A31" s="2"/>
       <c r="D31" t="s">
-        <v>16</v>
-      </c>
-      <c r="I31" t="s">
-        <v>114</v>
-      </c>
-      <c r="L31" t="b">
+        <v>15</v>
+      </c>
+      <c r="H31" t="s">
+        <v>153</v>
+      </c>
+      <c r="K31" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="12.75" customHeight="1">
+    <row r="32" spans="1:11" ht="12.75" customHeight="1">
       <c r="A32" s="2"/>
       <c r="D32" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G32" t="s">
+        <v>115</v>
+      </c>
+      <c r="H32" t="s">
         <v>113</v>
       </c>
-      <c r="E32" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="H32" t="s">
-        <v>117</v>
-      </c>
-      <c r="I32" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="33" spans="1:11" ht="12.75" customHeight="1">
       <c r="A33" s="2"/>
       <c r="D33" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G33" t="s">
+        <v>117</v>
+      </c>
+      <c r="H33" t="s">
         <v>118</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="H33" t="s">
-        <v>119</v>
-      </c>
-      <c r="I33" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="12.75" customHeight="1">
+    </row>
+    <row r="34" spans="1:11" ht="12.75" customHeight="1">
       <c r="A34" s="2"/>
       <c r="D34" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G34" t="s">
+        <v>120</v>
+      </c>
+      <c r="H34" t="s">
         <v>121</v>
       </c>
-      <c r="E34" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="H34" t="s">
+    </row>
+    <row r="35" spans="1:11" ht="12.75" customHeight="1">
+      <c r="A35" s="2"/>
+      <c r="B35" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="12.75" customHeight="1">
+      <c r="A36" s="2"/>
+      <c r="B36" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="12.75" customHeight="1">
+      <c r="A37" s="2"/>
+      <c r="D37" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" t="s">
+        <v>154</v>
+      </c>
+      <c r="K37" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="12.75" customHeight="1">
+      <c r="A38" s="2"/>
+      <c r="D38" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="I34" t="s">
+      <c r="E38" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G38" t="s">
+        <v>136</v>
+      </c>
+      <c r="H38" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="12.75" customHeight="1">
+      <c r="A39" s="2"/>
+      <c r="D39" s="6" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A35" s="2"/>
-      <c r="D35" s="6" t="s">
+      <c r="E39" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G39" t="s">
+        <v>137</v>
+      </c>
+      <c r="H39" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="12.75" customHeight="1">
+      <c r="A40" s="2"/>
+      <c r="D40" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="E35" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="H35" t="s">
+      <c r="E40" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G40" t="s">
         <v>138</v>
       </c>
-      <c r="I35" t="s">
+      <c r="H40" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A36" s="2"/>
-      <c r="D36" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="H36" t="s">
-        <v>139</v>
-      </c>
-      <c r="I36" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A37" s="2"/>
-      <c r="D37" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="H37" t="s">
-        <v>140</v>
-      </c>
-      <c r="I37" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="12.75" customHeight="1">
-      <c r="A38" s="2"/>
-      <c r="B38" s="4" t="s">
-        <v>21</v>
+    <row r="41" spans="1:11" ht="12.75" customHeight="1">
+      <c r="A41" s="2"/>
+      <c r="B41" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1424,7 +1462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -1435,272 +1473,272 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.75" customHeight="1">
       <c r="A1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" t="s">
         <v>97</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>98</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>99</v>
-      </c>
-      <c r="D1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16.75" customHeight="1">
       <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>46</v>
-      </c>
-      <c r="C2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.75" customHeight="1">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
         <v>48</v>
-      </c>
-      <c r="C3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.75" customHeight="1">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
         <v>50</v>
-      </c>
-      <c r="C4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.75" customHeight="1">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
         <v>52</v>
-      </c>
-      <c r="C5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.75" customHeight="1">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
         <v>54</v>
-      </c>
-      <c r="C6" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.75" customHeight="1">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
         <v>56</v>
-      </c>
-      <c r="C7" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16.75" customHeight="1">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" t="s">
         <v>58</v>
-      </c>
-      <c r="C8" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16.75" customHeight="1">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" t="s">
         <v>60</v>
-      </c>
-      <c r="C9" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16.75" customHeight="1">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" t="s">
         <v>62</v>
-      </c>
-      <c r="C10" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16.75" customHeight="1"/>
     <row r="12" spans="1:4" ht="16.75" customHeight="1">
       <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
         <v>64</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
         <v>65</v>
-      </c>
-      <c r="D12" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16.75" customHeight="1">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" t="s">
         <v>67</v>
-      </c>
-      <c r="D13" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16.75" customHeight="1"/>
     <row r="15" spans="1:4" ht="16.75" customHeight="1">
       <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" t="s">
         <v>69</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>70</v>
-      </c>
-      <c r="D15" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16.75" customHeight="1">
       <c r="A16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" t="s">
         <v>72</v>
-      </c>
-      <c r="D16" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16.75" customHeight="1">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" t="s">
         <v>74</v>
-      </c>
-      <c r="D17" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16.75" customHeight="1"/>
     <row r="19" spans="1:4" ht="12.75" customHeight="1">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="12.75" customHeight="1">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B20" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="12.75" customHeight="1">
       <c r="A21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B21" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="12.75" customHeight="1">
       <c r="A22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="12.75" customHeight="1">
       <c r="A24" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D24" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="12.75" customHeight="1">
       <c r="A25" t="s">
+        <v>125</v>
+      </c>
+      <c r="B25" t="s">
+        <v>132</v>
+      </c>
+      <c r="D25" t="s">
         <v>127</v>
-      </c>
-      <c r="B25" t="s">
-        <v>134</v>
-      </c>
-      <c r="D25" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="12.75" customHeight="1">
       <c r="A26" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B26" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D26" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="12.75" customHeight="1">
       <c r="A27" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B27" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="12.75" customHeight="1">
       <c r="A28" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B28" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D28" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1716,86 +1754,101 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.33203125" customWidth="1"/>
-    <col min="2" max="2" width="87.33203125" customWidth="1"/>
-    <col min="3" max="3" width="76.5" customWidth="1"/>
+    <col min="1" max="2" width="28.33203125" customWidth="1"/>
+    <col min="3" max="3" width="87.33203125" customWidth="1"/>
+    <col min="4" max="4" width="76.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="34.5" customHeight="1">
+    <row r="1" spans="1:4" ht="34.5" customHeight="1">
       <c r="A1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
         <v>76</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="34.5" customHeight="1">
+      <c r="A2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="34.5" customHeight="1">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" t="s">
         <v>78</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="34.5" customHeight="1">
+      <c r="A3" t="s">
         <v>79</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="34.5" customHeight="1">
+      <c r="A4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="34.5" customHeight="1">
-      <c r="A3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="34.5" customHeight="1">
-      <c r="A4" t="s">
+    <row r="5" spans="1:4" ht="34.5" customHeight="1">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" t="s">
         <v>82</v>
       </c>
-      <c r="B4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="34.5" customHeight="1">
-      <c r="A5" t="s">
+    <row r="6" spans="1:4" ht="34.5" customHeight="1">
+      <c r="A6" t="s">
         <v>84</v>
       </c>
-      <c r="B5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="34.5" customHeight="1">
-      <c r="A6" t="s">
+      <c r="C6" t="s">
         <v>85</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>86</v>
       </c>
-      <c r="C6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="16.25" customHeight="1"/>
+    </row>
+    <row r="7" spans="1:4" ht="16.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1821,27 +1874,27 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.75" customHeight="1">
       <c r="A1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16.75" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>90</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="16.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3">
         <v>20130408</v>
@@ -1849,10 +1902,10 @@
     </row>
     <row r="4" spans="1:3" ht="16.75" customHeight="1">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16.75" customHeight="1"/>

</xml_diff>

<commit_message>
Add functionality for commenting out lines in the xlsx forms to aid in form development
</commit_message>
<xml_diff>
--- a/form-files/tables/selects/forms/selects/selects.xlsx
+++ b/form-files/tables/selects/forms/selects/selects.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="4300" windowWidth="38040" windowHeight="21420" activeTab="2"/>
+    <workbookView xWindow="1800" yWindow="7880" windowWidth="38040" windowHeight="21420"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="154">
   <si>
     <t>comments</t>
   </si>
@@ -451,24 +451,6 @@
     <t>Christmas</t>
   </si>
   <si>
-    <t>thanksgiving</t>
-  </si>
-  <si>
-    <t>Thanksgiving</t>
-  </si>
-  <si>
-    <t>easter</t>
-  </si>
-  <si>
-    <t>Easter</t>
-  </si>
-  <si>
-    <t>halloween</t>
-  </si>
-  <si>
-    <t>Halloween</t>
-  </si>
-  <si>
     <t>query_type</t>
   </si>
   <si>
@@ -482,6 +464,39 @@
   </si>
   <si>
     <t>Food</t>
+  </si>
+  <si>
+    <t>kwanzaa</t>
+  </si>
+  <si>
+    <t>Kwanzaa</t>
+  </si>
+  <si>
+    <t>hannukah</t>
+  </si>
+  <si>
+    <t>Hannukah</t>
+  </si>
+  <si>
+    <t>Diwali</t>
+  </si>
+  <si>
+    <t>diwali</t>
+  </si>
+  <si>
+    <t>//if</t>
+  </si>
+  <si>
+    <t>//</t>
+  </si>
+  <si>
+    <t>// end if</t>
+  </si>
+  <si>
+    <t>//begin screen</t>
+  </si>
+  <si>
+    <t>//end screen</t>
   </si>
 </sst>
 </file>
@@ -916,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1185,7 +1200,7 @@
     <row r="21" spans="1:11" ht="15.75" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" s="4" t="s">
-        <v>95</v>
+        <v>149</v>
       </c>
       <c r="C21" t="s">
         <v>33</v>
@@ -1195,6 +1210,9 @@
       <c r="A22" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="B22" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="D22" t="s">
         <v>15</v>
       </c>
@@ -1208,7 +1226,7 @@
     <row r="23" spans="1:11" ht="15.75" customHeight="1">
       <c r="A23" s="2"/>
       <c r="B23" s="4" t="s">
-        <v>96</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1">
@@ -1265,16 +1283,19 @@
     <row r="27" spans="1:11" ht="12.75" customHeight="1">
       <c r="A27" s="2"/>
       <c r="B27" s="4" t="s">
-        <v>12</v>
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="12.75" customHeight="1">
       <c r="A28" s="2"/>
+      <c r="B28" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="D28" t="s">
         <v>15</v>
       </c>
       <c r="H28" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="K28" t="b">
         <v>1</v>
@@ -1282,6 +1303,9 @@
     </row>
     <row r="29" spans="1:11" ht="12.75" customHeight="1">
       <c r="A29" s="2"/>
+      <c r="B29" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="D29" s="6" t="s">
         <v>106</v>
       </c>
@@ -1297,6 +1321,9 @@
     </row>
     <row r="30" spans="1:11" ht="12.75" customHeight="1">
       <c r="A30" s="2"/>
+      <c r="B30" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="D30" s="6" t="s">
         <v>110</v>
       </c>
@@ -1312,6 +1339,9 @@
     </row>
     <row r="31" spans="1:11" ht="12.75" customHeight="1">
       <c r="A31" s="2"/>
+      <c r="B31" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="D31" s="6" t="s">
         <v>113</v>
       </c>
@@ -1328,7 +1358,7 @@
     <row r="32" spans="1:11" ht="12.75" customHeight="1">
       <c r="A32" s="2"/>
       <c r="B32" s="4" t="s">
-        <v>20</v>
+        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="12.75" customHeight="1">
@@ -1343,7 +1373,7 @@
         <v>15</v>
       </c>
       <c r="H34" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="K34" t="b">
         <v>1</v>
@@ -1416,7 +1446,7 @@
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1600,10 +1630,10 @@
         <v>108</v>
       </c>
       <c r="B19" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="D19" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="12.75" customHeight="1">
@@ -1611,10 +1641,10 @@
         <v>108</v>
       </c>
       <c r="B20" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D20" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="12.75" customHeight="1">
@@ -1622,10 +1652,10 @@
         <v>108</v>
       </c>
       <c r="B21" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="D21" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="12.75" customHeight="1">
@@ -1633,10 +1663,10 @@
         <v>108</v>
       </c>
       <c r="B22" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="D22" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="12.75" customHeight="1">
@@ -1709,7 +1739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1725,7 +1755,7 @@
         <v>89</v>
       </c>
       <c r="B1" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C1" t="s">
         <v>72</v>
@@ -1739,7 +1769,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
         <v>75</v>
@@ -1753,7 +1783,7 @@
         <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C3" t="s">
         <v>77</v>
@@ -1767,7 +1797,7 @@
         <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C4" t="s">
         <v>79</v>
@@ -1781,7 +1811,7 @@
         <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C5" t="s">
         <v>79</v>

</xml_diff>

<commit_message>
Change choice filter to use choice_item instead of context
</commit_message>
<xml_diff>
--- a/form-files/tables/selects/forms/selects/selects.xlsx
+++ b/form-files/tables/selects/forms/selects/selects.xlsx
@@ -144,9 +144,6 @@
     <t>Choose a region:</t>
   </si>
   <si>
-    <t>context.region === data('region')</t>
-  </si>
-  <si>
     <t>birds</t>
   </si>
   <si>
@@ -497,6 +494,9 @@
   </si>
   <si>
     <t>//end screen</t>
+  </si>
+  <si>
+    <t>choice_item.region === data('region')</t>
   </si>
 </sst>
 </file>
@@ -932,7 +932,7 @@
   <dimension ref="A1:K38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -953,7 +953,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
@@ -962,7 +962,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -971,16 +971,16 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
@@ -988,10 +988,10 @@
         <v>6</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G2" t="s">
         <v>7</v>
@@ -1003,10 +1003,10 @@
     <row r="3" spans="1:11" ht="15.75" customHeight="1">
       <c r="A3" s="2"/>
       <c r="D3" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G3" t="s">
         <v>9</v>
@@ -1026,10 +1026,10 @@
     <row r="5" spans="1:11" ht="15.75" customHeight="1">
       <c r="A5" s="2"/>
       <c r="D5" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G5" t="s">
         <v>13</v>
@@ -1041,7 +1041,7 @@
     <row r="6" spans="1:11" ht="15.75" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
@@ -1062,13 +1062,13 @@
     <row r="8" spans="1:11" ht="15.75" customHeight="1">
       <c r="A8" s="2"/>
       <c r="B8" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1">
       <c r="A9" s="2"/>
       <c r="B9" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -1089,7 +1089,7 @@
     <row r="11" spans="1:11" ht="15.75" customHeight="1">
       <c r="A11" s="2"/>
       <c r="B11" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
@@ -1119,10 +1119,10 @@
     <row r="15" spans="1:11" ht="15.75" customHeight="1">
       <c r="A15" s="2"/>
       <c r="D15" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G15" t="s">
         <v>22</v>
@@ -1134,10 +1134,10 @@
     <row r="16" spans="1:11" ht="15.75" customHeight="1">
       <c r="A16" s="2"/>
       <c r="D16" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G16" t="s">
         <v>24</v>
@@ -1149,10 +1149,10 @@
     <row r="17" spans="1:11" ht="15.75" customHeight="1">
       <c r="A17" s="2"/>
       <c r="D17" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G17" t="s">
         <v>26</v>
@@ -1164,10 +1164,10 @@
     <row r="18" spans="1:11" ht="15.75" customHeight="1">
       <c r="A18" s="2"/>
       <c r="D18" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G18" t="s">
         <v>28</v>
@@ -1185,10 +1185,10 @@
     <row r="20" spans="1:11" ht="15.75" customHeight="1">
       <c r="A20" s="2"/>
       <c r="D20" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G20" t="s">
         <v>30</v>
@@ -1200,7 +1200,7 @@
     <row r="21" spans="1:11" ht="15.75" customHeight="1">
       <c r="A21" s="2"/>
       <c r="B21" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C21" t="s">
         <v>33</v>
@@ -1211,7 +1211,7 @@
         <v>32</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D22" t="s">
         <v>15</v>
@@ -1226,16 +1226,16 @@
     <row r="23" spans="1:11" ht="15.75" customHeight="1">
       <c r="A23" s="2"/>
       <c r="B23" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1">
       <c r="A24" s="2"/>
       <c r="D24" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F24" t="s">
         <v>35</v>
@@ -1250,10 +1250,10 @@
     <row r="25" spans="1:11" ht="15.75" customHeight="1">
       <c r="A25" s="2"/>
       <c r="D25" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G25" t="s">
         <v>38</v>
@@ -1265,37 +1265,37 @@
     <row r="26" spans="1:11" ht="15.75" customHeight="1">
       <c r="A26" s="2"/>
       <c r="D26" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H26" t="s">
         <v>8</v>
       </c>
       <c r="J26" t="s">
-        <v>40</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="12.75" customHeight="1">
       <c r="A27" s="2"/>
       <c r="B27" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="12.75" customHeight="1">
       <c r="A28" s="2"/>
       <c r="B28" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D28" t="s">
         <v>15</v>
       </c>
       <c r="H28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K28" t="b">
         <v>1</v>
@@ -1304,61 +1304,61 @@
     <row r="29" spans="1:11" ht="12.75" customHeight="1">
       <c r="A29" s="2"/>
       <c r="B29" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D29" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G29" t="s">
+        <v>108</v>
+      </c>
+      <c r="H29" t="s">
         <v>106</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="G29" t="s">
-        <v>109</v>
-      </c>
-      <c r="H29" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="12.75" customHeight="1">
       <c r="A30" s="2"/>
       <c r="B30" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D30" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G30" t="s">
         <v>110</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>111</v>
-      </c>
-      <c r="H30" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="12.75" customHeight="1">
       <c r="A31" s="2"/>
       <c r="B31" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D31" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="G31" t="s">
         <v>113</v>
       </c>
-      <c r="E31" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>114</v>
-      </c>
-      <c r="H31" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="12.75" customHeight="1">
       <c r="A32" s="2"/>
       <c r="B32" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="12.75" customHeight="1">
@@ -1373,7 +1373,7 @@
         <v>15</v>
       </c>
       <c r="H34" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K34" t="b">
         <v>1</v>
@@ -1382,46 +1382,46 @@
     <row r="35" spans="1:11" ht="12.75" customHeight="1">
       <c r="A35" s="2"/>
       <c r="D35" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="12.75" customHeight="1">
       <c r="A36" s="2"/>
       <c r="D36" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="12.75" customHeight="1">
       <c r="A37" s="2"/>
       <c r="D37" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E37" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="E37" s="6" t="s">
-        <v>119</v>
-      </c>
       <c r="G37" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H37" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="12.75" customHeight="1">
@@ -1456,272 +1456,272 @@
   <sheetData>
     <row r="1" spans="1:4" ht="16.75" customHeight="1">
       <c r="A1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" t="s">
         <v>90</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>91</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>92</v>
-      </c>
-      <c r="D1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16.75" customHeight="1">
       <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>42</v>
-      </c>
-      <c r="C2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.75" customHeight="1">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
         <v>44</v>
-      </c>
-      <c r="C3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.75" customHeight="1">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
         <v>46</v>
-      </c>
-      <c r="C4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.75" customHeight="1">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
         <v>48</v>
-      </c>
-      <c r="C5" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.75" customHeight="1">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
         <v>50</v>
-      </c>
-      <c r="C6" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.75" customHeight="1">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" t="s">
         <v>52</v>
-      </c>
-      <c r="C7" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16.75" customHeight="1">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" t="s">
         <v>54</v>
-      </c>
-      <c r="C8" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16.75" customHeight="1">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
         <v>56</v>
-      </c>
-      <c r="C9" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16.75" customHeight="1">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" t="s">
         <v>58</v>
-      </c>
-      <c r="C10" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16.75" customHeight="1"/>
     <row r="12" spans="1:4" ht="16.75" customHeight="1">
       <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" t="s">
         <v>60</v>
       </c>
-      <c r="B12" t="s">
+      <c r="D12" t="s">
         <v>61</v>
-      </c>
-      <c r="D12" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="16.75" customHeight="1">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" t="s">
         <v>63</v>
-      </c>
-      <c r="D13" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16.75" customHeight="1"/>
     <row r="15" spans="1:4" ht="16.75" customHeight="1">
       <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
         <v>65</v>
       </c>
-      <c r="B15" t="s">
+      <c r="D15" t="s">
         <v>66</v>
-      </c>
-      <c r="D15" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16.75" customHeight="1">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" t="s">
         <v>68</v>
-      </c>
-      <c r="D16" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="16.75" customHeight="1">
       <c r="A17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" t="s">
         <v>70</v>
-      </c>
-      <c r="D17" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="16.75" customHeight="1"/>
     <row r="19" spans="1:4" ht="12.75" customHeight="1">
       <c r="A19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B19" t="s">
+        <v>142</v>
+      </c>
+      <c r="D19" t="s">
         <v>143</v>
-      </c>
-      <c r="D19" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="12.75" customHeight="1">
       <c r="A20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B20" t="s">
+        <v>135</v>
+      </c>
+      <c r="D20" t="s">
         <v>136</v>
-      </c>
-      <c r="D20" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="12.75" customHeight="1">
       <c r="A21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B21" t="s">
+        <v>144</v>
+      </c>
+      <c r="D21" t="s">
         <v>145</v>
-      </c>
-      <c r="D21" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="12.75" customHeight="1">
       <c r="A22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="12.75" customHeight="1">
       <c r="A24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" t="s">
         <v>119</v>
-      </c>
-      <c r="B24" t="s">
-        <v>125</v>
-      </c>
-      <c r="D24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="12.75" customHeight="1">
       <c r="A25" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="12.75" customHeight="1">
       <c r="A26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D26" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="12.75" customHeight="1">
       <c r="A27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D27" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="12.75" customHeight="1">
       <c r="A28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1752,72 +1752,72 @@
   <sheetData>
     <row r="1" spans="1:4" ht="34.5" customHeight="1">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
         <v>72</v>
-      </c>
-      <c r="D1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="34.5" customHeight="1">
       <c r="A2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" t="s">
         <v>74</v>
       </c>
-      <c r="B2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C2" t="s">
-        <v>75</v>
-      </c>
       <c r="D2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="34.5" customHeight="1">
       <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C3" t="s">
         <v>76</v>
       </c>
-      <c r="B3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C3" t="s">
-        <v>77</v>
-      </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="34.5" customHeight="1">
       <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" t="s">
         <v>78</v>
       </c>
-      <c r="B4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C4" t="s">
-        <v>79</v>
-      </c>
       <c r="D4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="34.5" customHeight="1">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.25" customHeight="1"/>
@@ -1847,27 +1847,27 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16.75" customHeight="1">
       <c r="A1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>86</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16.75" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>83</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="16.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3">
         <v>20130408</v>
@@ -1875,10 +1875,10 @@
     </row>
     <row r="4" spans="1:3" ht="16.75" customHeight="1">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16.75" customHeight="1"/>

</xml_diff>

<commit_message>
Changed the appearance of the Contents screen and fixed contents for Selects
</commit_message>
<xml_diff>
--- a/form-files/tables/selects/forms/selects/selects.xlsx
+++ b/form-files/tables/selects/forms/selects/selects.xlsx
@@ -692,8 +692,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="101">
+  <cellStyleXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -820,7 +822,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="101">
+  <cellStyles count="103">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -871,6 +873,7 @@
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -921,6 +924,7 @@
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1222,8 +1226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="D26" workbookViewId="0">
+      <selection activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -1978,6 +1982,9 @@
         <v>179</v>
       </c>
       <c r="I62" s="5"/>
+      <c r="K62" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="63" spans="1:15" ht="17.5" customHeight="1">
       <c r="A63" s="2"/>
@@ -1994,9 +2001,6 @@
       </c>
       <c r="I63" t="s">
         <v>169</v>
-      </c>
-      <c r="K63" t="b">
-        <v>1</v>
       </c>
       <c r="N63" t="s">
         <v>170</v>

</xml_diff>